<commit_message>
cleared new_template.xlsx, ready for new user
</commit_message>
<xml_diff>
--- a/WalkingApp/new_template.xlsx
+++ b/WalkingApp/new_template.xlsx
@@ -35,16 +35,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="177" formatCode="#,000_);[Red]\(#,000\)"/>
-    <numFmt numFmtId="178" formatCode="hh:mm:ss;@"/>
-    <numFmt numFmtId="179" formatCode="0.00;[Red]0.00"/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="#,000_);[Red]\(#,000\)"/>
+    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="h:mm;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -52,6 +50,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -71,17 +77,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -94,15 +101,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,17 +115,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,9 +151,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,21 +161,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,6 +176,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,7 +212,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +224,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +248,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +260,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +284,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,7 +302,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,109 +386,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,6 +411,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,15 +463,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -504,118 +502,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
@@ -624,57 +622,45 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -729,15 +715,6 @@
     <cellStyle name="Percent" xfId="47" builtinId="5"/>
     <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1005,13 +982,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD7"/>
+  <dimension ref="A1:XFD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G12" sqref="A2:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="12.4921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
@@ -17416,125 +17393,7 @@
       <c r="XFC1"/>
       <c r="XFD1"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7">
-        <v>45261</v>
-      </c>
-      <c r="B2" s="5">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8">
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="D2" s="6">
-        <v>548</v>
-      </c>
-      <c r="E2" s="6">
-        <v>9390</v>
-      </c>
-      <c r="G2"/>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="7">
-        <v>45262</v>
-      </c>
-      <c r="B3" s="5">
-        <v>8.38</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.0777083333333333</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1296</v>
-      </c>
-      <c r="E3" s="6">
-        <v>15540</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7">
-        <v>45263</v>
-      </c>
-      <c r="B4" s="5">
-        <v>12.74</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0.111111111111111</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1412</v>
-      </c>
-      <c r="E4" s="6">
-        <v>20071</v>
-      </c>
-      <c r="G4"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7">
-        <v>45264</v>
-      </c>
-      <c r="B5" s="5">
-        <v>14.92</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.135821759259259</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1782</v>
-      </c>
-      <c r="E5" s="6">
-        <v>23160</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7">
-        <v>45265</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3.78</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="D6" s="6">
-        <v>799</v>
-      </c>
-      <c r="E6" s="6">
-        <v>10224</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7">
-        <v>45266</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.0104166666666667</v>
-      </c>
-      <c r="D7" s="9">
-        <v>264</v>
-      </c>
-      <c r="E7" s="9">
-        <v>4838</v>
-      </c>
-      <c r="F7"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
-      <formula>20000</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>